<commit_message>
Proveedor Module Test Ok
</commit_message>
<xml_diff>
--- a/src/test/resources/CE-003.xlsx
+++ b/src/test/resources/CE-003.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CP-001" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="402">
   <si>
     <t xml:space="preserve">10714190321</t>
   </si>
@@ -541,6 +541,9 @@
     <t xml:space="preserve">Se muestra mensaje "El campo Monto total debe ser obligatorio"</t>
   </si>
   <si>
+    <t xml:space="preserve">80714080004</t>
+  </si>
+  <si>
     <t xml:space="preserve">Corporacion@gmail.com</t>
   </si>
   <si>
@@ -550,15 +553,24 @@
     <t xml:space="preserve">Proveedor creado con exito</t>
   </si>
   <si>
+    <t xml:space="preserve">80714080005</t>
+  </si>
+  <si>
     <t xml:space="preserve">Se muestra mensaje "El proveedor se registro con exito"</t>
   </si>
   <si>
+    <t xml:space="preserve">80714080006</t>
+  </si>
+  <si>
     <t xml:space="preserve">"Se muestra mensaje "El campo Razon Social no puede quedar vacio"" </t>
   </si>
   <si>
     <t xml:space="preserve">Se muestra el mensaje "Completa este campo" en el campo Razón Social</t>
   </si>
   <si>
+    <t xml:space="preserve">10714080006</t>
+  </si>
+  <si>
     <t xml:space="preserve">Se muestra mensaje "El campo Razon Social debe tener menos de 100 caracteres"</t>
   </si>
   <si>
@@ -566,6 +578,9 @@
   </si>
   <si>
     <t xml:space="preserve">Se muestra el mensaje "Haz conincidir el formato solicitado. Formato: 11 digitos"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80714080007</t>
   </si>
   <si>
     <t xml:space="preserve">Corporacion</t>
@@ -579,22 +594,34 @@
     <t xml:space="preserve">Se muestra el mensaje "Incluye un signo "@" en la direccion de correo electronico. La direccion "Coorporacion" no incluye el signo "@"".</t>
   </si>
   <si>
+    <t xml:space="preserve">80714080008</t>
+  </si>
+  <si>
     <t xml:space="preserve">Se muestra mensaje "El campo línea de crédito debe ser un numero mayor que 0"</t>
   </si>
   <si>
     <t xml:space="preserve">Se muestra el mensaje "El campo linea credito debe ser mayor que 0"</t>
   </si>
   <si>
+    <t xml:space="preserve">80714080009</t>
+  </si>
+  <si>
     <t xml:space="preserve">Se muestra mensaje "El campo línea de crédito debe ser un numero menor que 50000"</t>
   </si>
   <si>
     <t xml:space="preserve">Se muestra el mensaje "El campo linea credito debe ser menor igual que 49999"</t>
   </si>
   <si>
+    <t xml:space="preserve">80714080010</t>
+  </si>
+  <si>
     <t xml:space="preserve">Se muestra mensaje "El campo sobregiro debe ser un numero mayor que 0"</t>
   </si>
   <si>
     <t xml:space="preserve">Se muestra el mensaje "El campo sobregiro debe ser mayor igual que 0"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80714080011</t>
   </si>
   <si>
     <t xml:space="preserve">Se muestra mensaje "El campo sobregiro debe ser un numero menor que 10000"</t>
@@ -2826,7 +2853,7 @@
   </sheetPr>
   <dimension ref="A1:S1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -6989,8 +7016,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7010,11 +7037,11 @@
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="n">
-        <v>10714080003</v>
+      <c r="B1" s="1" t="s">
+        <v>165</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D1" s="2" t="n">
         <v>40000</v>
@@ -7023,21 +7050,21 @@
         <v>9000</v>
       </c>
       <c r="F1" s="70" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G1" s="71" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H1" s="72" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>10714080003</v>
+      <c r="B2" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="n">
@@ -7047,10 +7074,10 @@
         <v>9000</v>
       </c>
       <c r="F2" s="70" t="s">
+        <v>170</v>
+      </c>
+      <c r="G2" s="73" t="s">
         <v>168</v>
-      </c>
-      <c r="G2" s="73" t="s">
-        <v>167</v>
       </c>
       <c r="H2" s="72" t="s">
         <v>14</v>
@@ -7058,11 +7085,11 @@
     </row>
     <row r="3" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10"/>
-      <c r="B3" s="8" t="n">
-        <v>10714080003</v>
+      <c r="B3" s="8" t="s">
+        <v>171</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D3" s="10" t="n">
         <v>40000</v>
@@ -7071,10 +7098,10 @@
         <v>9000</v>
       </c>
       <c r="F3" s="74" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G3" s="75" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H3" s="72" t="s">
         <v>14</v>
@@ -7084,11 +7111,11 @@
       <c r="A4" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="8" t="n">
-        <v>10714080003</v>
+      <c r="B4" s="8" t="s">
+        <v>174</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D4" s="10" t="n">
         <v>40000</v>
@@ -7097,10 +7124,10 @@
         <v>9000</v>
       </c>
       <c r="F4" s="74" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="G4" s="74" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="H4" s="72" t="s">
         <v>14</v>
@@ -7115,7 +7142,7 @@
         <v>123456789</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D5" s="6" t="n">
         <v>40000</v>
@@ -7127,7 +7154,7 @@
         <v>22</v>
       </c>
       <c r="G5" s="77" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="H5" s="72" t="s">
         <v>14</v>
@@ -7141,7 +7168,7 @@
         <v>123451234512345</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D6" s="6" t="n">
         <v>40000</v>
@@ -7153,7 +7180,7 @@
         <v>22</v>
       </c>
       <c r="G6" s="77" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="H6" s="72" t="s">
         <v>14</v>
@@ -7163,11 +7190,11 @@
       <c r="A7" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="24" t="n">
-        <v>10714080003</v>
+      <c r="B7" s="24" t="s">
+        <v>178</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D7" s="25" t="n">
         <v>40000</v>
@@ -7176,10 +7203,10 @@
         <v>9000</v>
       </c>
       <c r="F7" s="78" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="G7" s="79" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="H7" s="72" t="s">
         <v>14</v>
@@ -7189,11 +7216,11 @@
       <c r="A8" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="49" t="n">
-        <v>10714080003</v>
+      <c r="B8" s="49" t="s">
+        <v>182</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D8" s="66" t="n">
         <v>-1000</v>
@@ -7202,10 +7229,10 @@
         <v>9000</v>
       </c>
       <c r="F8" s="80" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="G8" s="81" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="H8" s="72" t="s">
         <v>14</v>
@@ -7215,11 +7242,11 @@
       <c r="A9" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="49" t="n">
-        <v>10714080003</v>
+      <c r="B9" s="49" t="s">
+        <v>185</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D9" s="66" t="n">
         <v>65000</v>
@@ -7228,10 +7255,10 @@
         <v>9000</v>
       </c>
       <c r="F9" s="53" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="G9" s="81" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="H9" s="72" t="s">
         <v>14</v>
@@ -7242,11 +7269,11 @@
       <c r="A10" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="56" t="n">
-        <v>10714080003</v>
+      <c r="B10" s="56" t="s">
+        <v>188</v>
       </c>
       <c r="C10" s="55" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D10" s="55" t="n">
         <v>40000</v>
@@ -7255,10 +7282,10 @@
         <v>-2000</v>
       </c>
       <c r="F10" s="82" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="G10" s="83" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="H10" s="72" t="s">
         <v>14</v>
@@ -7268,11 +7295,11 @@
       <c r="A11" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="56" t="n">
-        <v>10714080003</v>
+      <c r="B11" s="56" t="s">
+        <v>191</v>
       </c>
       <c r="C11" s="55" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D11" s="55" t="n">
         <v>40000</v>
@@ -7281,10 +7308,10 @@
         <v>15000</v>
       </c>
       <c r="F11" s="60" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="G11" s="83" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="H11" s="72" t="s">
         <v>14</v>
@@ -8324,7 +8351,7 @@
         <v>1234567890123</v>
       </c>
       <c r="C1" s="85" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="D1" s="86" t="n">
         <v>1000</v>
@@ -8340,13 +8367,13 @@
         <v>12500</v>
       </c>
       <c r="H1" s="86" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="I1" s="89" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="J1" s="90" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="K1" s="91"/>
     </row>
@@ -8358,7 +8385,7 @@
         <v>1234566543321</v>
       </c>
       <c r="C2" s="85" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="D2" s="86" t="n">
         <v>2000</v>
@@ -8374,13 +8401,13 @@
         <v>25028</v>
       </c>
       <c r="H2" s="86" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="I2" s="89" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="J2" s="93" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="K2" s="36"/>
     </row>
@@ -8392,7 +8419,7 @@
         <v>1234567890123</v>
       </c>
       <c r="C3" s="96" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="D3" s="96" t="n">
         <v>1000</v>
@@ -8408,13 +8435,13 @@
         <v>12500</v>
       </c>
       <c r="H3" s="96" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="I3" s="100" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="J3" s="101" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="K3" s="12"/>
       <c r="L3" s="102"/>
@@ -8427,7 +8454,7 @@
         <v>1234566543321</v>
       </c>
       <c r="C4" s="96" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="D4" s="96" t="n">
         <v>2000</v>
@@ -8443,13 +8470,13 @@
         <v>25028</v>
       </c>
       <c r="H4" s="96" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="I4" s="100" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="J4" s="101" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="K4" s="12"/>
     </row>
@@ -8461,7 +8488,7 @@
         <v>123456789</v>
       </c>
       <c r="C5" s="106" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="D5" s="106" t="n">
         <v>1000</v>
@@ -8477,13 +8504,13 @@
         <v>12500</v>
       </c>
       <c r="H5" s="106" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="I5" s="106" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="J5" s="110" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="K5" s="36"/>
     </row>
@@ -8495,7 +8522,7 @@
         <v>123456789123456</v>
       </c>
       <c r="C6" s="106" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="D6" s="106" t="n">
         <v>2000</v>
@@ -8511,13 +8538,13 @@
         <v>25028</v>
       </c>
       <c r="H6" s="106" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="I6" s="106" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="J6" s="113" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="K6" s="36"/>
     </row>
@@ -8544,10 +8571,10 @@
       </c>
       <c r="H7" s="79"/>
       <c r="I7" s="118" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="J7" s="119" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="K7" s="4"/>
     </row>
@@ -8559,7 +8586,7 @@
         <v>1234567890123</v>
       </c>
       <c r="C8" s="121" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="D8" s="122" t="n">
         <v>900</v>
@@ -8575,13 +8602,13 @@
         <v>11250</v>
       </c>
       <c r="H8" s="121" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="I8" s="80" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="J8" s="126" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="K8" s="36"/>
     </row>
@@ -8593,7 +8620,7 @@
         <v>1234566543321</v>
       </c>
       <c r="C9" s="121" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="D9" s="122" t="n">
         <v>6000</v>
@@ -8609,13 +8636,13 @@
         <v>75084</v>
       </c>
       <c r="H9" s="121" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="I9" s="53" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="J9" s="129" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="K9" s="36"/>
     </row>
@@ -8627,7 +8654,7 @@
         <v>1234567890123</v>
       </c>
       <c r="C10" s="86" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="D10" s="86" t="n">
         <v>1000</v>
@@ -8643,13 +8670,13 @@
         <v>12525</v>
       </c>
       <c r="H10" s="86" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="I10" s="131" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="J10" s="132" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="K10" s="36"/>
     </row>
@@ -8661,7 +8688,7 @@
         <v>1234566543321</v>
       </c>
       <c r="C11" s="86" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="D11" s="86" t="n">
         <v>2000</v>
@@ -8677,13 +8704,13 @@
         <v>25029.308</v>
       </c>
       <c r="H11" s="86" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="I11" s="131" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="J11" s="132" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="K11" s="36"/>
     </row>
@@ -8695,7 +8722,7 @@
         <v>1234567890123</v>
       </c>
       <c r="C12" s="96" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="D12" s="96" t="n">
         <v>2000</v>
@@ -8711,16 +8738,16 @@
         <v>25028.24</v>
       </c>
       <c r="H12" s="96" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="I12" s="137" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="J12" s="54" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8731,7 +8758,7 @@
         <v>1234566543321</v>
       </c>
       <c r="C13" s="96" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="D13" s="96" t="n">
         <v>2000</v>
@@ -8747,16 +8774,16 @@
         <v>25028.24</v>
       </c>
       <c r="H13" s="96" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="I13" s="137" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="J13" s="54" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8767,7 +8794,7 @@
         <v>1234566543321</v>
       </c>
       <c r="C14" s="106" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="D14" s="106" t="n">
         <v>2000</v>
@@ -8780,7 +8807,7 @@
       </c>
       <c r="G14" s="138"/>
       <c r="H14" s="106" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="I14" s="45" t="s">
         <v>164</v>
@@ -8798,7 +8825,7 @@
         <v>1234566543321</v>
       </c>
       <c r="C15" s="79" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="D15" s="79" t="n">
         <v>2000</v>
@@ -8815,7 +8842,7 @@
       </c>
       <c r="H15" s="141"/>
       <c r="I15" s="118" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="J15" s="118" t="s">
         <v>146</v>
@@ -9843,7 +9870,7 @@
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C2" s="72"/>
       <c r="D2" s="143" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="E2" s="143"/>
       <c r="G2" s="4"/>
@@ -9851,49 +9878,49 @@
     </row>
     <row r="3" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="144" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="B3" s="144" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="C3" s="144" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="D3" s="145" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="E3" s="145" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="F3" s="144" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="G3" s="144" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="H3" s="142"/>
     </row>
     <row r="4" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="146" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="B4" s="147" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="C4" s="148" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>123456</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="G4" s="70" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="H4" s="142" t="s">
         <v>14</v>
@@ -9901,25 +9928,25 @@
     </row>
     <row r="5" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="149" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="B5" s="150" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="C5" s="151" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="E5" s="7" t="n">
         <v>123456</v>
       </c>
       <c r="F5" s="39" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="G5" s="39" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="H5" s="142" t="s">
         <v>14</v>
@@ -9927,23 +9954,23 @@
     </row>
     <row r="6" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="149" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="B6" s="150" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="C6" s="151" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="7" t="n">
         <v>12345</v>
       </c>
       <c r="F6" s="39" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="G6" s="39" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="H6" s="142" t="s">
         <v>14</v>
@@ -9951,25 +9978,25 @@
     </row>
     <row r="7" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="152" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="B7" s="153" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="C7" s="154" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="E7" s="155" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="F7" s="75" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="G7" s="74" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="H7" s="142" t="s">
         <v>14</v>
@@ -9977,26 +10004,26 @@
     </row>
     <row r="8" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="152" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="B8" s="153" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="C8" s="154" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="75" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="G8" s="74" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="H8" s="142" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -11020,86 +11047,86 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C2" s="157" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="D2" s="157"/>
       <c r="E2" s="157" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c r="F2" s="157"/>
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="157" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="B3" s="157" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="C3" s="157" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="D3" s="157" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="E3" s="157" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="F3" s="157" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="158" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c r="B4" s="158" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C4" s="159" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="D4" s="160" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="E4" s="161" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="F4" s="158" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="158"/>
       <c r="B5" s="158"/>
       <c r="C5" s="162" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="D5" s="160"/>
       <c r="E5" s="161" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="F5" s="158" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="158" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="B6" s="158" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C6" s="163" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="D6" s="160" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="E6" s="161" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="F6" s="158" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11108,105 +11135,105 @@
       <c r="C7" s="164"/>
       <c r="D7" s="160"/>
       <c r="E7" s="161" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="F7" s="158" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="158" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="B8" s="158" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C8" s="163" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="D8" s="160" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="E8" s="165" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="F8" s="158" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="158"/>
       <c r="B9" s="158"/>
       <c r="C9" s="163" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="D9" s="160"/>
       <c r="E9" s="161" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="F9" s="158" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="158" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="B10" s="158" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C10" s="163" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="D10" s="160" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="E10" s="161" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="F10" s="158" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="158"/>
       <c r="B11" s="158"/>
       <c r="C11" s="163" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="D11" s="160"/>
       <c r="E11" s="161" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="F11" s="158" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="158" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="B12" s="158" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C12" s="163" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="D12" s="160" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="E12" s="161" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="F12" s="158" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="158"/>
       <c r="B13" s="158"/>
       <c r="C13" s="163" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="D13" s="160"/>
       <c r="E13" s="161"/>
@@ -11214,77 +11241,77 @@
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="158" t="s">
-        <v>280</v>
+        <v>289</v>
       </c>
       <c r="B14" s="158" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C14" s="163" t="s">
-        <v>281</v>
+        <v>290</v>
       </c>
       <c r="D14" s="160" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="E14" s="161" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
       <c r="F14" s="158" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="158"/>
       <c r="B15" s="158"/>
       <c r="C15" s="163" t="s">
-        <v>284</v>
+        <v>293</v>
       </c>
       <c r="D15" s="160"/>
       <c r="E15" s="161" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="F15" s="158" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="158"/>
       <c r="B16" s="158"/>
       <c r="C16" s="163" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="D16" s="160"/>
       <c r="E16" s="161" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="F16" s="158" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="158" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="B17" s="158" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C17" s="163" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="D17" s="160" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="E17" s="161" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="F17" s="158" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="158"/>
       <c r="B18" s="158"/>
       <c r="C18" s="163" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="D18" s="160"/>
       <c r="E18" s="161"/>
@@ -11292,56 +11319,56 @@
     </row>
     <row r="19" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="158" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="B19" s="158" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C19" s="163" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="D19" s="166" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
       <c r="E19" s="161" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
       <c r="F19" s="158" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="158"/>
       <c r="B20" s="158"/>
       <c r="C20" s="163" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="D20" s="166"/>
       <c r="E20" s="161" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
       <c r="F20" s="158" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="158" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
       <c r="B21" s="158" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C21" s="163" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
       <c r="D21" s="160" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="E21" s="161" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="F21" s="158" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11350,30 +11377,30 @@
       <c r="C22" s="164"/>
       <c r="D22" s="160"/>
       <c r="E22" s="161" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="F22" s="158" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="158" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="B23" s="158" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C23" s="163" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="D23" s="166" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
       <c r="E23" s="161" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="F23" s="158" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11382,30 +11409,30 @@
       <c r="C24" s="164"/>
       <c r="D24" s="166"/>
       <c r="E24" s="161" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
       <c r="F24" s="158" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="158" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
       <c r="B25" s="158" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C25" s="163" t="s">
-        <v>314</v>
+        <v>323</v>
       </c>
       <c r="D25" s="160" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="E25" s="161" t="s">
-        <v>315</v>
+        <v>324</v>
       </c>
       <c r="F25" s="158" t="s">
-        <v>316</v>
+        <v>325</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11414,30 +11441,30 @@
       <c r="C26" s="164"/>
       <c r="D26" s="160"/>
       <c r="E26" s="161" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
       <c r="F26" s="158" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="158" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="B27" s="158" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C27" s="163" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
       <c r="D27" s="160" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="E27" s="161" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
       <c r="F27" s="158" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11446,10 +11473,10 @@
       <c r="C28" s="167"/>
       <c r="D28" s="160"/>
       <c r="E28" s="161" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="F28" s="158" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11458,30 +11485,30 @@
       <c r="C29" s="162"/>
       <c r="D29" s="160"/>
       <c r="E29" s="161" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="F29" s="158" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="158" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
       <c r="B30" s="158" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C30" s="163" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
       <c r="D30" s="166" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
       <c r="E30" s="161" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
       <c r="F30" s="158" t="s">
-        <v>328</v>
+        <v>337</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11490,71 +11517,71 @@
       <c r="C31" s="164"/>
       <c r="D31" s="166"/>
       <c r="E31" s="161" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="F31" s="158" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="158" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="B32" s="158" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C32" s="168" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="D32" s="160" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="E32" s="169" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="F32" s="158" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="158"/>
       <c r="B33" s="158"/>
       <c r="C33" s="168" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="D33" s="160"/>
       <c r="E33" s="169" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="F33" s="158" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="158" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="B34" s="158" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C34" s="163" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="D34" s="160" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="E34" s="161" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="F34" s="158" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="158"/>
       <c r="B35" s="158"/>
       <c r="C35" s="163" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="D35" s="160"/>
       <c r="E35" s="161"/>
@@ -11562,7 +11589,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="156" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
       <c r="B38" s="156"/>
       <c r="C38" s="156"/>
@@ -11572,86 +11599,86 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C39" s="157" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="D39" s="157"/>
       <c r="E39" s="157" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c r="F39" s="157"/>
     </row>
     <row r="40" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="157" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="B40" s="157" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="C40" s="157" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="D40" s="157" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="E40" s="157" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="F40" s="157" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="158" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
       <c r="B41" s="158" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C41" s="170" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
       <c r="D41" s="160" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="E41" s="161" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="F41" s="171" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="158"/>
       <c r="B42" s="158"/>
       <c r="C42" s="172" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="D42" s="160"/>
       <c r="E42" s="161" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="F42" s="173" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="158" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="B43" s="158" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C43" s="170" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="D43" s="166" t="s">
-        <v>347</v>
+        <v>356</v>
       </c>
       <c r="E43" s="170" t="s">
-        <v>348</v>
+        <v>357</v>
       </c>
       <c r="F43" s="173" t="s">
-        <v>349</v>
+        <v>358</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11660,62 +11687,62 @@
       <c r="C44" s="161"/>
       <c r="D44" s="166"/>
       <c r="E44" s="170" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="F44" s="173" t="s">
-        <v>351</v>
+        <v>360</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="158" t="s">
-        <v>352</v>
+        <v>361</v>
       </c>
       <c r="B45" s="158" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="C45" s="170" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="D45" s="160" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="E45" s="165" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="F45" s="173" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="158"/>
       <c r="B46" s="158"/>
       <c r="C46" s="170" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="D46" s="160"/>
       <c r="E46" s="161" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="F46" s="173" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="158" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="B47" s="158" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C47" s="170" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
       <c r="D47" s="166"/>
       <c r="E47" s="170" t="s">
-        <v>357</v>
+        <v>366</v>
       </c>
       <c r="F47" s="173" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11724,30 +11751,30 @@
       <c r="C48" s="161"/>
       <c r="D48" s="166"/>
       <c r="E48" s="170" t="s">
-        <v>358</v>
+        <v>367</v>
       </c>
       <c r="F48" s="173" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="158" t="s">
-        <v>359</v>
+        <v>368</v>
       </c>
       <c r="B49" s="158" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C49" s="170" t="s">
-        <v>360</v>
+        <v>369</v>
       </c>
       <c r="D49" s="160" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="E49" s="170" t="s">
-        <v>361</v>
+        <v>370</v>
       </c>
       <c r="F49" s="173" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11756,30 +11783,30 @@
       <c r="C50" s="161"/>
       <c r="D50" s="160"/>
       <c r="E50" s="170" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
       <c r="F50" s="173" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="158" t="s">
+        <v>372</v>
+      </c>
+      <c r="B51" s="158" t="s">
+        <v>310</v>
+      </c>
+      <c r="C51" s="161" t="s">
+        <v>373</v>
+      </c>
+      <c r="D51" s="160" t="s">
+        <v>261</v>
+      </c>
+      <c r="E51" s="161" t="s">
         <v>363</v>
       </c>
-      <c r="B51" s="158" t="s">
-        <v>301</v>
-      </c>
-      <c r="C51" s="161" t="s">
-        <v>364</v>
-      </c>
-      <c r="D51" s="160" t="s">
-        <v>252</v>
-      </c>
-      <c r="E51" s="161" t="s">
-        <v>354</v>
-      </c>
       <c r="F51" s="173" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="1.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11800,22 +11827,22 @@
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="158" t="s">
-        <v>365</v>
+        <v>374</v>
       </c>
       <c r="B54" s="158" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
       <c r="C54" s="161" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="D54" s="160" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="E54" s="161" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="F54" s="158" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11828,7 +11855,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="156" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
       <c r="B58" s="156"/>
       <c r="C58" s="156"/>
@@ -11838,82 +11865,82 @@
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C59" s="157" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="D59" s="157"/>
       <c r="E59" s="157" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c r="F59" s="157"/>
     </row>
     <row r="60" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="144" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="B60" s="144" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="C60" s="144" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="D60" s="144" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="E60" s="144" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="F60" s="144" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="158" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
       <c r="B61" s="158" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C61" s="174" t="s">
-        <v>370</v>
+        <v>379</v>
       </c>
       <c r="D61" s="166"/>
       <c r="E61" s="174" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
       <c r="F61" s="158" t="s">
-        <v>372</v>
+        <v>381</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="158"/>
       <c r="B62" s="158"/>
       <c r="C62" s="172" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="D62" s="166"/>
       <c r="E62" s="161" t="s">
-        <v>373</v>
+        <v>382</v>
       </c>
       <c r="F62" s="158" t="s">
-        <v>374</v>
+        <v>383</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="158" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
       <c r="B63" s="158" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C63" s="161" t="s">
-        <v>376</v>
+        <v>385</v>
       </c>
       <c r="D63" s="166"/>
       <c r="E63" s="161" t="s">
-        <v>377</v>
+        <v>386</v>
       </c>
       <c r="F63" s="158" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11922,108 +11949,108 @@
       <c r="C64" s="175"/>
       <c r="D64" s="166"/>
       <c r="E64" s="161" t="s">
-        <v>378</v>
+        <v>387</v>
       </c>
       <c r="F64" s="158" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="158" t="s">
-        <v>379</v>
+        <v>388</v>
       </c>
       <c r="B65" s="158" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C65" s="161" t="s">
-        <v>380</v>
+        <v>389</v>
       </c>
       <c r="D65" s="160"/>
       <c r="E65" s="161" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
       <c r="F65" s="158" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="158"/>
       <c r="B66" s="158"/>
       <c r="C66" s="161" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="D66" s="160"/>
       <c r="E66" s="161" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="F66" s="158" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="158" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="B67" s="158" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C67" s="161" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
       <c r="D67" s="166"/>
       <c r="E67" s="161" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
       <c r="F67" s="158" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="158"/>
       <c r="B68" s="158"/>
       <c r="C68" s="161" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="D68" s="166"/>
       <c r="E68" s="161" t="s">
-        <v>388</v>
+        <v>397</v>
       </c>
       <c r="F68" s="158" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="158" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="B69" s="158" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C69" s="161" t="s">
-        <v>390</v>
+        <v>399</v>
       </c>
       <c r="D69" s="160" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="E69" s="161" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
       <c r="F69" s="158" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="158"/>
       <c r="B70" s="158"/>
       <c r="C70" s="161" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="D70" s="160"/>
       <c r="E70" s="161" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
       <c r="F70" s="158" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>